<commit_message>
update after - 1st web page practice - github.com
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -7,7 +7,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TECH" sheetId="1" r:id="rId1"/>
+    <sheet name="INFRA" sheetId="2" r:id="rId2"/>
+    <sheet name="WEB DESIGN" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>PYTHON</t>
   </si>
@@ -39,9 +41,6 @@
     <t>ADHOC</t>
   </si>
   <si>
-    <t>Regular Espression</t>
-  </si>
-  <si>
     <t>html5 &amp; css3</t>
   </si>
   <si>
@@ -139,13 +138,107 @@
   </si>
   <si>
     <t>Angular JS</t>
+  </si>
+  <si>
+    <t>JAVA HOSTING SERVICES</t>
+  </si>
+  <si>
+    <t>https://www.heroku.com/</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/appengine/</t>
+  </si>
+  <si>
+    <t>https://www.openshift.com/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/</t>
+  </si>
+  <si>
+    <t>https://www.rosehosting.com/</t>
+  </si>
+  <si>
+    <t>https://console.cloud.google.com/start</t>
+  </si>
+  <si>
+    <t>Why UTF-8 is used?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common questions </t>
+  </si>
+  <si>
+    <t>https://github.com/</t>
+  </si>
+  <si>
+    <t>https://www.xoom.com/india/mobile-reloads</t>
+  </si>
+  <si>
+    <t>https://moodle.com/</t>
+  </si>
+  <si>
+    <t>PRACTICE EXAMPLES</t>
+  </si>
+  <si>
+    <t>CMS</t>
+  </si>
+  <si>
+    <t>Moodle</t>
+  </si>
+  <si>
+    <t>Wordpress</t>
+  </si>
+  <si>
+    <t>Joomla</t>
+  </si>
+  <si>
+    <t>i18N</t>
+  </si>
+  <si>
+    <t>Regular Expression</t>
+  </si>
+  <si>
+    <t>In how many different ways can you show list menu horizontally</t>
+  </si>
+  <si>
+    <t>li</t>
+  </si>
+  <si>
+    <t>display:inline</t>
+  </si>
+  <si>
+    <t>ul</t>
+  </si>
+  <si>
+    <t>list-style:none</t>
+  </si>
+  <si>
+    <t>float:left</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>What are the different ways of uploading a file to server ?</t>
+  </si>
+  <si>
+    <t>How to know which jars are in runtime.</t>
+  </si>
+  <si>
+    <t>What is Base 64 encoding?</t>
+  </si>
+  <si>
+    <t>What are the different ways
+ of encryption?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,8 +270,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +305,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -215,27 +319,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -565,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -580,12 +714,12 @@
     <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.83203125" customWidth="1"/>
     <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -597,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -609,118 +743,299 @@
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30">
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K7"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>19</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" t="s">
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D4" s="4">
+        <v>147821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:10">
+      <c r="C2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10">
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10">
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="F11" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>